<commit_message>
This code is the latest till 30 June for AndroidTestCases
</commit_message>
<xml_diff>
--- a/TestData/A9951E20.xlsx
+++ b/TestData/A9951E20.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AFF040B-92CF-4BEB-8734-B114F6E4EBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EF0747-4DD9-4F38-B7E1-4D521E1D14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
   <si>
     <t>995859</t>
   </si>
@@ -63,25 +63,7 @@
     <t>110091</t>
   </si>
   <si>
-    <t>Invalid Full Name</t>
-  </si>
-  <si>
     <t>Invalid Email</t>
-  </si>
-  <si>
-    <t>Invalid DOB</t>
-  </si>
-  <si>
-    <t>Invalid Address</t>
-  </si>
-  <si>
-    <t>Invalid Pincode</t>
-  </si>
-  <si>
-    <t>Abhay@0000001</t>
-  </si>
-  <si>
-    <t>ABCD</t>
   </si>
   <si>
     <t>Valid_fullName</t>
@@ -177,9 +159,6 @@
     <t>abcd123&amp;#*$()</t>
   </si>
   <si>
-    <t>f30mumbaibandraeast+++++++@#%^^&amp;%^*!@#$@#$%^*^(</t>
-  </si>
-  <si>
     <t>2537461014</t>
   </si>
   <si>
@@ -192,18 +171,12 @@
     <t>Please check your network connection.</t>
   </si>
   <si>
-    <t>1/2/23</t>
-  </si>
-  <si>
     <t>1/2/01</t>
   </si>
   <si>
     <t>Personal vaild details (Under my profile)</t>
   </si>
   <si>
-    <t>Personal invaild details (Under my profile)</t>
-  </si>
-  <si>
     <t>Personal details page (Expected results)</t>
   </si>
   <si>
@@ -279,9 +252,6 @@
     <t>PIN Code</t>
   </si>
   <si>
-    <t>000000</t>
-  </si>
-  <si>
     <t>Goodlife member mob number</t>
   </si>
   <si>
@@ -307,6 +277,15 @@
   </si>
   <si>
     <t>6666600011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gunjanrawatGmail.</t>
+  </si>
+  <si>
+    <t>!@!@222</t>
+  </si>
+  <si>
+    <t>01-02-2001</t>
   </si>
 </sst>
 </file>
@@ -378,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -410,6 +389,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,7 +743,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -772,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -780,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -793,10 +773,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -850,24 +830,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -885,10 +865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,7 +879,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -908,7 +888,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -950,134 +930,110 @@
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="11"/>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
+      <c r="B11" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
+      <c r="B12" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
+      <c r="A20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" t="s">
-        <v>80</v>
+        <v>54</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>82</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{1E98206A-73D5-4A8D-94B1-7EF178E5E015}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{1526CF94-F6A9-4F64-9F94-C88E5E5C3A03}"/>
-    <hyperlink ref="B23" r:id="rId3" xr:uid="{559745FE-7564-41C2-9E82-584DD90D55A4}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{4D44F7CC-98F6-4F7D-866D-3D2B9745655B}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{559745FE-7564-41C2-9E82-584DD90D55A4}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{4D44F7CC-98F6-4F7D-866D-3D2B9745655B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1098,108 +1054,108 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1207,10 +1163,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1239,30 +1195,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1291,62 +1247,62 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1378,16 +1334,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to execute the appium server programatically in BaseClass
</commit_message>
<xml_diff>
--- a/TestData/A9951E20.xlsx
+++ b/TestData/A9951E20.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EF0747-4DD9-4F38-B7E1-4D521E1D14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECC9A9D-A41D-4C7C-AF9A-5803791FE465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -276,9 +276,6 @@
     <t>goodlife member</t>
   </si>
   <si>
-    <t>6666600011</t>
-  </si>
-  <si>
     <t xml:space="preserve"> gunjanrawatGmail.</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>01-02-2001</t>
+  </si>
+  <si>
+    <t>7777777777</t>
   </si>
 </sst>
 </file>
@@ -377,6 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,7 +390,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,9 +409,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -449,9 +449,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,26 +484,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,26 +519,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -731,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,17 +708,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -829,10 +795,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -851,8 +817,8 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -867,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -878,10 +844,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -933,8 +899,8 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>85</v>
+      <c r="B9" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -944,12 +910,12 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -970,10 +936,10 @@
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
@@ -1053,10 +1019,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1091,10 +1057,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1121,10 +1087,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
@@ -1194,10 +1160,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1208,10 +1174,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1246,10 +1212,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1276,10 +1242,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1333,10 +1299,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>